<commit_message>
changed duration data to seconds, made graphs more attractive, added exploratory analysis of duration vs hr
</commit_message>
<xml_diff>
--- a/hr_data.xlsx
+++ b/hr_data.xlsx
@@ -341,7 +341,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -359,7 +359,7 @@
         <v>146.0</v>
       </c>
       <c r="E2" s="1">
-        <v>30.15</v>
+        <v>1815.0</v>
       </c>
     </row>
     <row r="3">
@@ -376,9 +376,9 @@
         <v>154.0</v>
       </c>
       <c r="E3" s="1">
-        <v>29.43</v>
-      </c>
-      <c r="F3" s="1" t="s">
+        <v>1783.0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -396,9 +396,9 @@
         <v>128.0</v>
       </c>
       <c r="E4" s="1">
-        <v>14.07</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>847.0</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -416,7 +416,7 @@
         <v>146.0</v>
       </c>
       <c r="E5" s="1">
-        <v>30.07</v>
+        <v>1807.0</v>
       </c>
     </row>
     <row r="6">
@@ -433,9 +433,9 @@
         <v>137.0</v>
       </c>
       <c r="E6" s="1">
-        <v>30.14</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>1814.0</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -453,7 +453,7 @@
         <v>140.0</v>
       </c>
       <c r="E7" s="1">
-        <v>30.16</v>
+        <v>1816.0</v>
       </c>
     </row>
     <row r="8">
@@ -470,9 +470,9 @@
         <v>130.0</v>
       </c>
       <c r="E8" s="1">
-        <v>21.2</v>
-      </c>
-      <c r="F8" s="1" t="s">
+        <v>1280.0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -490,9 +490,9 @@
         <v>143.0</v>
       </c>
       <c r="E9" s="1">
-        <v>31.29</v>
-      </c>
-      <c r="F9" s="1" t="s">
+        <v>1889.0</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -510,9 +510,9 @@
         <v>154.0</v>
       </c>
       <c r="E10" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="F10" s="1" t="s">
+        <v>1920.0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -530,9 +530,9 @@
         <v>125.0</v>
       </c>
       <c r="E11" s="1">
-        <v>19.07</v>
-      </c>
-      <c r="F11" s="1" t="s">
+        <v>1147.0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -550,9 +550,9 @@
         <v>148.0</v>
       </c>
       <c r="E12" s="1">
-        <v>32.14</v>
-      </c>
-      <c r="F12" s="1" t="s">
+        <v>1934.0</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -570,9 +570,9 @@
         <v>136.0</v>
       </c>
       <c r="E13" s="1">
-        <v>14.37</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>877.0</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -590,9 +590,9 @@
         <v>142.0</v>
       </c>
       <c r="E14" s="1">
-        <v>32.17</v>
-      </c>
-      <c r="F14" s="1" t="s">
+        <v>1937.0</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -610,9 +610,9 @@
         <v>152.0</v>
       </c>
       <c r="E15" s="1">
-        <v>30.15</v>
-      </c>
-      <c r="F15" s="1" t="s">
+        <v>1635.0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>